<commit_message>
added track no 4
</commit_message>
<xml_diff>
--- a/AVR 음악 주파수.xlsx
+++ b/AVR 음악 주파수.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WinAVR-RTOS\avr_rtos_orgel_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D763E9E0-8A72-4690-BCF5-BE285943020A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85847B11-2289-4454-AC1B-B3319D87360B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14976" activeTab="3" xr2:uid="{2A465206-010F-4655-81D6-FB1FD6055048}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14976" activeTab="4" xr2:uid="{2A465206-010F-4655-81D6-FB1FD6055048}"/>
   </bookViews>
   <sheets>
     <sheet name="코드표" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="236">
   <si>
     <t>B8</t>
   </si>
@@ -859,6 +859,58 @@
   </si>
   <si>
     <t>노트길이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G#4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A#4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>key_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>note_size</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -9403,8 +9455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37FA565B-722B-41B4-AC68-8ECC1B03CA2F}">
   <dimension ref="A1:F154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C154"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -11874,462 +11926,2843 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8B1577-E6D3-4CED-ABFA-BC6DADF1001D}">
-  <dimension ref="A1:A90"/>
+  <dimension ref="A1:D236"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <f>VLOOKUP(A2,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <f>VLOOKUP(A3,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <f>VLOOKUP(A4,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <f>VLOOKUP(A5,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f>VLOOKUP(A6,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f>VLOOKUP(A7,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <f>VLOOKUP(A8,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f>VLOOKUP(A9,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f>VLOOKUP(A10,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f>VLOOKUP(A11,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <f>VLOOKUP(A12,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <f>VLOOKUP(A13,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f>VLOOKUP(A14,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f>VLOOKUP(A15,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <f>VLOOKUP(A16,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <f>VLOOKUP(A17,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <f>VLOOKUP(A18,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <f>VLOOKUP(A19,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <f>VLOOKUP(A20,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <f>VLOOKUP(A21,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <f>VLOOKUP(A22,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
+        <v>207</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f>VLOOKUP(A23,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>206</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <f>VLOOKUP(A24,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <f>VLOOKUP(A25,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <f>VLOOKUP(A26,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
+        <v>205</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <f>VLOOKUP(A27,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <f>VLOOKUP(A28,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <f>VLOOKUP(A29,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
+        <v>206</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <f>VLOOKUP(A30,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>207</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <f>VLOOKUP(A31,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <f>VLOOKUP(A32,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>206</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <f>VLOOKUP(A33,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <f>VLOOKUP(A34,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>210</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <f>VLOOKUP(A35,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <f>VLOOKUP(A36,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <f>VLOOKUP(A37,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
+        <v>205</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <f>VLOOKUP(A38,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>206</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <f>VLOOKUP(A39,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <f>VLOOKUP(A40,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>205</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <f>VLOOKUP(A41,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <f>VLOOKUP(A42,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>203</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <f>VLOOKUP(A43,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <f>VLOOKUP(A44,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <f>VLOOKUP(A45,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
+        <v>204</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <f>VLOOKUP(A46,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>211</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <f>VLOOKUP(A47,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="D48">
+        <f>VLOOKUP(A48,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.4">
+        <v>212</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="D49">
+        <f>VLOOKUP(A49,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
+        <v>206</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <f>VLOOKUP(A50,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B51">
+        <v>13</v>
+      </c>
+      <c r="D51">
+        <f>VLOOKUP(A51,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.4">
+        <v>201</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="D52">
+        <f>VLOOKUP(A52,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
+        <v>200</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="D53">
+        <f>VLOOKUP(A53,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A54" t="s">
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <f>VLOOKUP(A54,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A55" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <f>VLOOKUP(A55,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <f>VLOOKUP(A56,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <f>VLOOKUP(A57,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
+        <v>203</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <f>VLOOKUP(A58,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
+        <v>204</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <f>VLOOKUP(A59,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
+        <v>205</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <f>VLOOKUP(A60,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A61" t="s">
+        <v>206</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="D61">
+        <f>VLOOKUP(A61,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A62" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A59" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A60" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A61" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A62" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B62">
+        <v>6</v>
+      </c>
+      <c r="D62">
+        <f>VLOOKUP(A62,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <f>VLOOKUP(A63,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.4">
+        <v>207</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="D64">
+        <f>VLOOKUP(A64,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.4">
+        <v>208</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <f>VLOOKUP(A65,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.4">
+        <v>209</v>
+      </c>
+      <c r="B66">
+        <v>4</v>
+      </c>
+      <c r="D66">
+        <f>VLOOKUP(A66,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B67">
+        <v>6</v>
+      </c>
+      <c r="D67">
+        <f>VLOOKUP(A67,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.4">
+        <v>213</v>
+      </c>
+      <c r="B68">
+        <v>4</v>
+      </c>
+      <c r="D68">
+        <f>VLOOKUP(A68,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
+        <v>214</v>
+      </c>
+      <c r="B69">
+        <v>4</v>
+      </c>
+      <c r="D69">
+        <f>VLOOKUP(A69,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A70" t="s">
+        <v>215</v>
+      </c>
+      <c r="B70">
+        <v>4</v>
+      </c>
+      <c r="D70">
+        <f>VLOOKUP(A70,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A71" t="s">
+        <v>202</v>
+      </c>
+      <c r="B71">
+        <v>4</v>
+      </c>
+      <c r="D71">
+        <f>VLOOKUP(A71,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A72" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72">
+        <v>4</v>
+      </c>
+      <c r="D72">
+        <f>VLOOKUP(A72,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A73" t="s">
+        <v>207</v>
+      </c>
+      <c r="B73">
+        <v>4</v>
+      </c>
+      <c r="D73">
+        <f>VLOOKUP(A73,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A74" t="s">
+        <v>202</v>
+      </c>
+      <c r="B74">
+        <v>8</v>
+      </c>
+      <c r="D74">
+        <f>VLOOKUP(A74,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A75" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A70" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A71" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A72" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A73" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A74" t="s">
+      <c r="B75">
+        <v>4</v>
+      </c>
+      <c r="D75">
+        <f>VLOOKUP(A75,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A76" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A75" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A76" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B76">
+        <v>4</v>
+      </c>
+      <c r="D76">
+        <f>VLOOKUP(A76,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.4">
+        <v>206</v>
+      </c>
+      <c r="B77">
+        <v>4</v>
+      </c>
+      <c r="D77">
+        <f>VLOOKUP(A77,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B78">
+        <v>4</v>
+      </c>
+      <c r="D78">
+        <f>VLOOKUP(A78,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
+        <v>141</v>
+      </c>
+      <c r="B79">
+        <v>4</v>
+      </c>
+      <c r="D79">
+        <f>VLOOKUP(A79,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A80" t="s">
+        <v>140</v>
+      </c>
+      <c r="B80">
+        <v>4</v>
+      </c>
+      <c r="D80">
+        <f>VLOOKUP(A80,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A81" t="s">
+        <v>170</v>
+      </c>
+      <c r="B81">
+        <v>8</v>
+      </c>
+      <c r="D81">
+        <f>VLOOKUP(A81,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A82" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A80" t="s">
+      <c r="B82">
+        <v>4</v>
+      </c>
+      <c r="D82">
+        <f>VLOOKUP(A82,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A83" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A81" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A82" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A83" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B83">
+        <v>4</v>
+      </c>
+      <c r="D83">
+        <f>VLOOKUP(A83,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.4">
+        <v>141</v>
+      </c>
+      <c r="B84">
+        <v>4</v>
+      </c>
+      <c r="D84">
+        <f>VLOOKUP(A84,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.4">
+        <v>170</v>
+      </c>
+      <c r="B85">
+        <v>4</v>
+      </c>
+      <c r="D85">
+        <f>VLOOKUP(A85,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.4">
+        <v>223</v>
+      </c>
+      <c r="B86">
+        <v>4</v>
+      </c>
+      <c r="D86">
+        <f>VLOOKUP(A86,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
+        <v>224</v>
+      </c>
+      <c r="B87">
+        <v>4</v>
+      </c>
+      <c r="D87">
+        <f>VLOOKUP(A87,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A88" t="s">
+        <v>226</v>
+      </c>
+      <c r="B88">
+        <v>8</v>
+      </c>
+      <c r="D88">
+        <f>VLOOKUP(A88,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A89" t="s">
+        <v>140</v>
+      </c>
+      <c r="B89">
+        <v>4</v>
+      </c>
+      <c r="D89">
+        <f>VLOOKUP(A89,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A90" t="s">
+        <v>225</v>
+      </c>
+      <c r="B90">
+        <v>2</v>
+      </c>
+      <c r="D90">
+        <f>VLOOKUP(A90,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A91" t="s">
+        <v>226</v>
+      </c>
+      <c r="B91">
+        <v>2</v>
+      </c>
+      <c r="D91">
+        <f>VLOOKUP(A91,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A92" t="s">
+        <v>223</v>
+      </c>
+      <c r="B92">
+        <v>4</v>
+      </c>
+      <c r="D92">
+        <f>VLOOKUP(A92,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A93" t="s">
+        <v>226</v>
+      </c>
+      <c r="B93">
+        <v>4</v>
+      </c>
+      <c r="D93">
+        <f>VLOOKUP(A93,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A94" t="s">
+        <v>227</v>
+      </c>
+      <c r="B94">
+        <v>4</v>
+      </c>
+      <c r="D94">
+        <f>VLOOKUP(A94,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A95" t="s">
+        <v>228</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <f>VLOOKUP(A95,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A96" t="s">
+        <v>226</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <f>VLOOKUP(A96,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A97" t="s">
+        <v>228</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <f>VLOOKUP(A97,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A98" t="s">
+        <v>229</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <f>VLOOKUP(A98,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A99" t="s">
+        <v>230</v>
+      </c>
+      <c r="B99">
+        <v>3</v>
+      </c>
+      <c r="D99">
+        <f>VLOOKUP(A99,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A100" t="s">
+        <v>226</v>
+      </c>
+      <c r="B100">
+        <v>5</v>
+      </c>
+      <c r="D100">
+        <f>VLOOKUP(A100,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A101" t="s">
+        <v>231</v>
+      </c>
+      <c r="B101">
+        <v>4</v>
+      </c>
+      <c r="D101">
+        <f>VLOOKUP(A101,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A102" t="s">
+        <v>225</v>
+      </c>
+      <c r="B102">
+        <v>8</v>
+      </c>
+      <c r="D102">
+        <f>VLOOKUP(A102,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A103" t="s">
+        <v>226</v>
+      </c>
+      <c r="B103">
+        <v>12</v>
+      </c>
+      <c r="D103">
+        <f>VLOOKUP(A103,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A104" t="s">
+        <v>201</v>
+      </c>
+      <c r="B104">
+        <v>4</v>
+      </c>
+      <c r="D104">
+        <f>VLOOKUP(A104,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A105" t="s">
+        <v>148</v>
+      </c>
+      <c r="B105">
+        <v>4</v>
+      </c>
+      <c r="D105">
+        <f>VLOOKUP(A105,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A106" t="s">
+        <v>170</v>
+      </c>
+      <c r="B106">
+        <v>2</v>
+      </c>
+      <c r="D106">
+        <f>VLOOKUP(A106,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A107" t="s">
+        <v>201</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <f>VLOOKUP(A107,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A108" t="s">
+        <v>170</v>
+      </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
+      <c r="D108">
+        <f>VLOOKUP(A108,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A109" t="s">
+        <v>201</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+      <c r="D109">
+        <f>VLOOKUP(A109,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A110" t="s">
+        <v>203</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="D110">
+        <f>VLOOKUP(A110,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A111" t="s">
+        <v>143</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="D111">
+        <f>VLOOKUP(A111,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A112" t="s">
+        <v>142</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+      <c r="D112">
+        <f>VLOOKUP(A112,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A113" t="s">
+        <v>141</v>
+      </c>
+      <c r="B113">
+        <v>4</v>
+      </c>
+      <c r="D113">
+        <f>VLOOKUP(A113,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A114" t="s">
+        <v>170</v>
+      </c>
+      <c r="B114">
+        <v>6</v>
+      </c>
+      <c r="D114">
+        <f>VLOOKUP(A114,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A115" t="s">
+        <v>141</v>
+      </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
+      <c r="D115">
+        <f>VLOOKUP(A115,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A116" t="s">
+        <v>140</v>
+      </c>
+      <c r="B116">
+        <v>2</v>
+      </c>
+      <c r="D116">
+        <f>VLOOKUP(A116,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A117" t="s">
+        <v>139</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
+      <c r="D117">
+        <f>VLOOKUP(A117,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A118" t="s">
+        <v>209</v>
+      </c>
+      <c r="B118">
+        <v>4</v>
+      </c>
+      <c r="D118">
+        <f>VLOOKUP(A118,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A119" t="s">
+        <v>170</v>
+      </c>
+      <c r="B119">
+        <v>5</v>
+      </c>
+      <c r="D119">
+        <f>VLOOKUP(A119,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A120" t="s">
+        <v>209</v>
+      </c>
+      <c r="B120">
+        <v>2</v>
+      </c>
+      <c r="D120">
+        <f>VLOOKUP(A120,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A121" t="s">
+        <v>139</v>
+      </c>
+      <c r="B121">
+        <v>2</v>
+      </c>
+      <c r="D121">
+        <f>VLOOKUP(A121,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A122" t="s">
+        <v>140</v>
+      </c>
+      <c r="B122">
+        <v>2</v>
+      </c>
+      <c r="D122">
+        <f>VLOOKUP(A122,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A123" t="s">
+        <v>139</v>
+      </c>
+      <c r="B123">
+        <v>4</v>
+      </c>
+      <c r="D123">
+        <f>VLOOKUP(A123,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A124" t="s">
+        <v>140</v>
+      </c>
+      <c r="B124">
+        <v>1</v>
+      </c>
+      <c r="D124">
+        <f>VLOOKUP(A124,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A125" t="s">
+        <v>141</v>
+      </c>
+      <c r="B125">
+        <v>2</v>
+      </c>
+      <c r="D125">
+        <f>VLOOKUP(A125,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A126" t="s">
+        <v>170</v>
+      </c>
+      <c r="B126">
+        <v>6</v>
+      </c>
+      <c r="D126">
+        <f>VLOOKUP(A126,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A127" t="s">
+        <v>141</v>
+      </c>
+      <c r="B127">
+        <v>3</v>
+      </c>
+      <c r="D127">
+        <f>VLOOKUP(A127,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A128" t="s">
+        <v>142</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
+      <c r="D128">
+        <f>VLOOKUP(A128,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A129" t="s">
+        <v>170</v>
+      </c>
+      <c r="B129">
+        <v>1</v>
+      </c>
+      <c r="D129">
+        <f>VLOOKUP(A129,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A130" t="s">
+        <v>142</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
+      <c r="D130">
+        <f>VLOOKUP(A130,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A131" t="s">
+        <v>141</v>
+      </c>
+      <c r="B131">
+        <v>1</v>
+      </c>
+      <c r="D131">
+        <f>VLOOKUP(A131,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A132" t="s">
+        <v>140</v>
+      </c>
+      <c r="B132">
+        <v>3</v>
+      </c>
+      <c r="D132">
+        <f>VLOOKUP(A132,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A133" t="s">
+        <v>170</v>
+      </c>
+      <c r="B133">
+        <v>4</v>
+      </c>
+      <c r="D133">
+        <f>VLOOKUP(A133,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A134" t="s">
+        <v>141</v>
+      </c>
+      <c r="B134">
+        <v>2</v>
+      </c>
+      <c r="D134">
+        <f>VLOOKUP(A134,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A135" t="s">
+        <v>142</v>
+      </c>
+      <c r="B135">
+        <v>2</v>
+      </c>
+      <c r="D135">
+        <f>VLOOKUP(A135,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A136" t="s">
+        <v>144</v>
+      </c>
+      <c r="B136">
+        <v>1</v>
+      </c>
+      <c r="D136">
+        <f>VLOOKUP(A136,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A137" t="s">
+        <v>170</v>
+      </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
+      <c r="D137">
+        <f>VLOOKUP(A137,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A138" t="s">
+        <v>144</v>
+      </c>
+      <c r="B138">
+        <v>1</v>
+      </c>
+      <c r="D138">
+        <f>VLOOKUP(A138,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A139" t="s">
+        <v>142</v>
+      </c>
+      <c r="B139">
+        <v>1</v>
+      </c>
+      <c r="D139">
+        <f>VLOOKUP(A139,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A140" t="s">
+        <v>141</v>
+      </c>
+      <c r="B140">
+        <v>3</v>
+      </c>
+      <c r="D140">
+        <f>VLOOKUP(A140,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A141" t="s">
+        <v>170</v>
+      </c>
+      <c r="B141">
+        <v>4</v>
+      </c>
+      <c r="D141">
+        <f>VLOOKUP(A141,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A142" t="s">
+        <v>142</v>
+      </c>
+      <c r="B142">
+        <v>2</v>
+      </c>
+      <c r="D142">
+        <f>VLOOKUP(A142,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A143" t="s">
+        <v>144</v>
+      </c>
+      <c r="B143">
+        <v>2</v>
+      </c>
+      <c r="D143">
+        <f>VLOOKUP(A143,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A144" t="s">
+        <v>203</v>
+      </c>
+      <c r="B144">
+        <v>1</v>
+      </c>
+      <c r="D144">
+        <f>VLOOKUP(A144,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A145" t="s">
+        <v>170</v>
+      </c>
+      <c r="B145">
+        <v>1</v>
+      </c>
+      <c r="D145">
+        <f>VLOOKUP(A145,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A146" t="s">
+        <v>203</v>
+      </c>
+      <c r="B146">
+        <v>1</v>
+      </c>
+      <c r="D146">
+        <f>VLOOKUP(A146,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A147" t="s">
+        <v>143</v>
+      </c>
+      <c r="B147">
+        <v>1</v>
+      </c>
+      <c r="D147">
+        <f>VLOOKUP(A147,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A148" t="s">
+        <v>211</v>
+      </c>
+      <c r="B148">
+        <v>3</v>
+      </c>
+      <c r="D148">
+        <f>VLOOKUP(A148,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A149" t="s">
+        <v>170</v>
+      </c>
+      <c r="B149">
+        <v>4</v>
+      </c>
+      <c r="D149">
+        <f>VLOOKUP(A149,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A150" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A88" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A89" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A90" t="s">
-        <v>204</v>
+      <c r="B150">
+        <v>4</v>
+      </c>
+      <c r="D150">
+        <f>VLOOKUP(A150,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A151" t="s">
+        <v>141</v>
+      </c>
+      <c r="B151">
+        <v>4</v>
+      </c>
+      <c r="D151">
+        <f>VLOOKUP(A151,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A152" t="s">
+        <v>170</v>
+      </c>
+      <c r="B152">
+        <v>13</v>
+      </c>
+      <c r="D152">
+        <f>VLOOKUP(A152,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A153" t="s">
+        <v>201</v>
+      </c>
+      <c r="B153">
+        <v>4</v>
+      </c>
+      <c r="D153">
+        <f>VLOOKUP(A153,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A154" t="s">
+        <v>148</v>
+      </c>
+      <c r="B154">
+        <v>4</v>
+      </c>
+      <c r="D154">
+        <f>VLOOKUP(A154,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A155" t="s">
+        <v>170</v>
+      </c>
+      <c r="B155">
+        <v>2</v>
+      </c>
+      <c r="D155">
+        <f>VLOOKUP(A155,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A156" t="s">
+        <v>201</v>
+      </c>
+      <c r="B156">
+        <v>1</v>
+      </c>
+      <c r="D156">
+        <f>VLOOKUP(A156,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A157" t="s">
+        <v>170</v>
+      </c>
+      <c r="B157">
+        <v>1</v>
+      </c>
+      <c r="D157">
+        <f>VLOOKUP(A157,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A158" t="s">
+        <v>201</v>
+      </c>
+      <c r="B158">
+        <v>1</v>
+      </c>
+      <c r="D158">
+        <f>VLOOKUP(A158,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A159" t="s">
+        <v>203</v>
+      </c>
+      <c r="B159">
+        <v>1</v>
+      </c>
+      <c r="D159">
+        <f>VLOOKUP(A159,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A160" t="s">
+        <v>143</v>
+      </c>
+      <c r="B160">
+        <v>1</v>
+      </c>
+      <c r="D160">
+        <f>VLOOKUP(A160,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A161" t="s">
+        <v>142</v>
+      </c>
+      <c r="B161">
+        <v>1</v>
+      </c>
+      <c r="D161">
+        <f>VLOOKUP(A161,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A162" t="s">
+        <v>141</v>
+      </c>
+      <c r="B162">
+        <v>4</v>
+      </c>
+      <c r="D162">
+        <f>VLOOKUP(A162,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A163" t="s">
+        <v>170</v>
+      </c>
+      <c r="B163">
+        <v>6</v>
+      </c>
+      <c r="D163">
+        <f>VLOOKUP(A163,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A164" t="s">
+        <v>141</v>
+      </c>
+      <c r="B164">
+        <v>1</v>
+      </c>
+      <c r="D164">
+        <f>VLOOKUP(A164,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A165" t="s">
+        <v>140</v>
+      </c>
+      <c r="B165">
+        <v>2</v>
+      </c>
+      <c r="D165">
+        <f>VLOOKUP(A165,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A166" t="s">
+        <v>139</v>
+      </c>
+      <c r="B166">
+        <v>1</v>
+      </c>
+      <c r="D166">
+        <f>VLOOKUP(A166,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A167" t="s">
+        <v>209</v>
+      </c>
+      <c r="B167">
+        <v>4</v>
+      </c>
+      <c r="D167">
+        <f>VLOOKUP(A167,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A168" t="s">
+        <v>170</v>
+      </c>
+      <c r="B168">
+        <v>6</v>
+      </c>
+      <c r="D168">
+        <f>VLOOKUP(A168,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A169" t="s">
+        <v>137</v>
+      </c>
+      <c r="B169">
+        <v>4</v>
+      </c>
+      <c r="D169">
+        <f>VLOOKUP(A169,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A170" t="s">
+        <v>214</v>
+      </c>
+      <c r="B170">
+        <v>4</v>
+      </c>
+      <c r="D170">
+        <f>VLOOKUP(A170,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A171" t="s">
+        <v>215</v>
+      </c>
+      <c r="B171">
+        <v>4</v>
+      </c>
+      <c r="D171">
+        <f>VLOOKUP(A171,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A172" t="s">
+        <v>170</v>
+      </c>
+      <c r="B172">
+        <v>4</v>
+      </c>
+      <c r="D172">
+        <f>VLOOKUP(A172,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A173" t="s">
+        <v>141</v>
+      </c>
+      <c r="B173">
+        <v>4</v>
+      </c>
+      <c r="D173">
+        <f>VLOOKUP(A173,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A174" t="s">
+        <v>140</v>
+      </c>
+      <c r="B174">
+        <v>4</v>
+      </c>
+      <c r="D174">
+        <f>VLOOKUP(A174,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A175" t="s">
+        <v>170</v>
+      </c>
+      <c r="B175">
+        <v>8</v>
+      </c>
+      <c r="D175">
+        <f>VLOOKUP(A175,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A176" t="s">
+        <v>209</v>
+      </c>
+      <c r="B176">
+        <v>4</v>
+      </c>
+      <c r="D176">
+        <f>VLOOKUP(A176,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A177" t="s">
+        <v>215</v>
+      </c>
+      <c r="B177">
+        <v>4</v>
+      </c>
+      <c r="D177">
+        <f>VLOOKUP(A177,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A178" t="s">
+        <v>141</v>
+      </c>
+      <c r="B178">
+        <v>4</v>
+      </c>
+      <c r="D178">
+        <f>VLOOKUP(A178,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A179" t="s">
+        <v>170</v>
+      </c>
+      <c r="B179">
+        <v>4</v>
+      </c>
+      <c r="D179">
+        <f>VLOOKUP(A179,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A180" t="s">
+        <v>141</v>
+      </c>
+      <c r="B180">
+        <v>4</v>
+      </c>
+      <c r="D180">
+        <f>VLOOKUP(A180,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A181" t="s">
+        <v>140</v>
+      </c>
+      <c r="B181">
+        <v>4</v>
+      </c>
+      <c r="D181">
+        <f>VLOOKUP(A181,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A182" t="s">
+        <v>170</v>
+      </c>
+      <c r="B182">
+        <v>8</v>
+      </c>
+      <c r="D182">
+        <f>VLOOKUP(A182,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A183" t="s">
+        <v>209</v>
+      </c>
+      <c r="B183">
+        <v>4</v>
+      </c>
+      <c r="D183">
+        <f>VLOOKUP(A183,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A184" t="s">
+        <v>215</v>
+      </c>
+      <c r="B184">
+        <v>4</v>
+      </c>
+      <c r="D184">
+        <f>VLOOKUP(A184,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A185" t="s">
+        <v>141</v>
+      </c>
+      <c r="B185">
+        <v>4</v>
+      </c>
+      <c r="D185">
+        <f>VLOOKUP(A185,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A186" t="s">
+        <v>170</v>
+      </c>
+      <c r="B186">
+        <v>4</v>
+      </c>
+      <c r="D186">
+        <f>VLOOKUP(A186,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A187" t="s">
+        <v>223</v>
+      </c>
+      <c r="B187">
+        <v>4</v>
+      </c>
+      <c r="D187">
+        <f>VLOOKUP(A187,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A188" t="s">
+        <v>224</v>
+      </c>
+      <c r="B188">
+        <v>4</v>
+      </c>
+      <c r="D188">
+        <f>VLOOKUP(A188,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A189" t="s">
+        <v>226</v>
+      </c>
+      <c r="B189">
+        <v>8</v>
+      </c>
+      <c r="D189">
+        <f>VLOOKUP(A189,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A190" t="s">
+        <v>140</v>
+      </c>
+      <c r="B190">
+        <v>4</v>
+      </c>
+      <c r="D190">
+        <f>VLOOKUP(A190,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A191" t="s">
+        <v>225</v>
+      </c>
+      <c r="B191">
+        <v>2</v>
+      </c>
+      <c r="D191">
+        <f>VLOOKUP(A191,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A192" t="s">
+        <v>226</v>
+      </c>
+      <c r="B192">
+        <v>2</v>
+      </c>
+      <c r="D192">
+        <f>VLOOKUP(A192,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A193" t="s">
+        <v>223</v>
+      </c>
+      <c r="B193">
+        <v>4</v>
+      </c>
+      <c r="D193">
+        <f>VLOOKUP(A193,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A194" t="s">
+        <v>226</v>
+      </c>
+      <c r="B194">
+        <v>4</v>
+      </c>
+      <c r="D194">
+        <f>VLOOKUP(A194,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A195" t="s">
+        <v>227</v>
+      </c>
+      <c r="B195">
+        <v>4</v>
+      </c>
+      <c r="D195">
+        <f>VLOOKUP(A195,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A196" t="s">
+        <v>228</v>
+      </c>
+      <c r="B196">
+        <v>1</v>
+      </c>
+      <c r="D196">
+        <f>VLOOKUP(A196,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A197" t="s">
+        <v>226</v>
+      </c>
+      <c r="B197">
+        <v>1</v>
+      </c>
+      <c r="D197">
+        <f>VLOOKUP(A197,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A198" t="s">
+        <v>228</v>
+      </c>
+      <c r="B198">
+        <v>1</v>
+      </c>
+      <c r="D198">
+        <f>VLOOKUP(A198,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A199" t="s">
+        <v>229</v>
+      </c>
+      <c r="B199">
+        <v>1</v>
+      </c>
+      <c r="D199">
+        <f>VLOOKUP(A199,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A200" t="s">
+        <v>230</v>
+      </c>
+      <c r="B200">
+        <v>3</v>
+      </c>
+      <c r="D200">
+        <f>VLOOKUP(A200,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A201" t="s">
+        <v>226</v>
+      </c>
+      <c r="B201">
+        <v>5</v>
+      </c>
+      <c r="D201">
+        <f>VLOOKUP(A201,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A202" t="s">
+        <v>231</v>
+      </c>
+      <c r="B202">
+        <v>4</v>
+      </c>
+      <c r="D202">
+        <f>VLOOKUP(A202,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A203" t="s">
+        <v>225</v>
+      </c>
+      <c r="B203">
+        <v>8</v>
+      </c>
+      <c r="D203">
+        <f>VLOOKUP(A203,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A204" t="s">
+        <v>226</v>
+      </c>
+      <c r="B204">
+        <v>10</v>
+      </c>
+      <c r="D204">
+        <f>VLOOKUP(A204,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A205" t="s">
+        <v>231</v>
+      </c>
+      <c r="B205">
+        <v>4</v>
+      </c>
+      <c r="D205">
+        <f>VLOOKUP(A205,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A206" t="s">
+        <v>226</v>
+      </c>
+      <c r="B206">
+        <v>4</v>
+      </c>
+      <c r="D206">
+        <f>VLOOKUP(A206,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A207" t="s">
+        <v>231</v>
+      </c>
+      <c r="B207">
+        <v>4</v>
+      </c>
+      <c r="D207">
+        <f>VLOOKUP(A207,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A208" t="s">
+        <v>226</v>
+      </c>
+      <c r="B208">
+        <v>4</v>
+      </c>
+      <c r="D208">
+        <f>VLOOKUP(A208,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A209" t="s">
+        <v>231</v>
+      </c>
+      <c r="B209">
+        <v>4</v>
+      </c>
+      <c r="D209">
+        <f>VLOOKUP(A209,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A210" t="s">
+        <v>226</v>
+      </c>
+      <c r="B210">
+        <v>8</v>
+      </c>
+      <c r="D210">
+        <f>VLOOKUP(A210,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A211" t="s">
+        <v>225</v>
+      </c>
+      <c r="B211">
+        <v>4</v>
+      </c>
+      <c r="D211">
+        <f>VLOOKUP(A211,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A212" t="s">
+        <v>231</v>
+      </c>
+      <c r="B212">
+        <v>4</v>
+      </c>
+      <c r="D212">
+        <f>VLOOKUP(A212,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A213" t="s">
+        <v>226</v>
+      </c>
+      <c r="B213">
+        <v>4</v>
+      </c>
+      <c r="D213">
+        <f>VLOOKUP(A213,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A214" t="s">
+        <v>231</v>
+      </c>
+      <c r="B214">
+        <v>4</v>
+      </c>
+      <c r="D214">
+        <f>VLOOKUP(A214,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A215" t="s">
+        <v>226</v>
+      </c>
+      <c r="B215">
+        <v>4</v>
+      </c>
+      <c r="D215">
+        <f>VLOOKUP(A215,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A216" t="s">
+        <v>231</v>
+      </c>
+      <c r="B216">
+        <v>4</v>
+      </c>
+      <c r="D216">
+        <f>VLOOKUP(A216,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A217" t="s">
+        <v>226</v>
+      </c>
+      <c r="B217">
+        <v>4</v>
+      </c>
+      <c r="D217">
+        <f>VLOOKUP(A217,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A218" t="s">
+        <v>232</v>
+      </c>
+      <c r="B218">
+        <v>2</v>
+      </c>
+      <c r="D218">
+        <f>VLOOKUP(A218,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A219" t="s">
+        <v>226</v>
+      </c>
+      <c r="B219">
+        <v>2</v>
+      </c>
+      <c r="D219">
+        <f>VLOOKUP(A219,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A220" t="s">
+        <v>232</v>
+      </c>
+      <c r="B220">
+        <v>2</v>
+      </c>
+      <c r="D220">
+        <f>VLOOKUP(A220,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A221" t="s">
+        <v>226</v>
+      </c>
+      <c r="B221">
+        <v>2</v>
+      </c>
+      <c r="D221">
+        <f>VLOOKUP(A221,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A222" t="s">
+        <v>231</v>
+      </c>
+      <c r="B222">
+        <v>4</v>
+      </c>
+      <c r="D222">
+        <f>VLOOKUP(A222,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A223" t="s">
+        <v>226</v>
+      </c>
+      <c r="B223">
+        <v>4</v>
+      </c>
+      <c r="D223">
+        <f>VLOOKUP(A223,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A224" t="s">
+        <v>231</v>
+      </c>
+      <c r="B224">
+        <v>4</v>
+      </c>
+      <c r="D224">
+        <f>VLOOKUP(A224,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A225" t="s">
+        <v>226</v>
+      </c>
+      <c r="B225">
+        <v>4</v>
+      </c>
+      <c r="D225">
+        <f>VLOOKUP(A225,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A226" t="s">
+        <v>231</v>
+      </c>
+      <c r="B226">
+        <v>4</v>
+      </c>
+      <c r="D226">
+        <f>VLOOKUP(A226,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A227" t="s">
+        <v>226</v>
+      </c>
+      <c r="B227">
+        <v>8</v>
+      </c>
+      <c r="D227">
+        <f>VLOOKUP(A227,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A228" t="s">
+        <v>225</v>
+      </c>
+      <c r="B228">
+        <v>4</v>
+      </c>
+      <c r="D228">
+        <f>VLOOKUP(A228,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A229" t="s">
+        <v>231</v>
+      </c>
+      <c r="B229">
+        <v>4</v>
+      </c>
+      <c r="D229">
+        <f>VLOOKUP(A229,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A230" t="s">
+        <v>226</v>
+      </c>
+      <c r="B230">
+        <v>4</v>
+      </c>
+      <c r="D230">
+        <f>VLOOKUP(A230,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A231" t="s">
+        <v>231</v>
+      </c>
+      <c r="B231">
+        <v>4</v>
+      </c>
+      <c r="D231">
+        <f>VLOOKUP(A231,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A232" t="s">
+        <v>226</v>
+      </c>
+      <c r="B232">
+        <v>4</v>
+      </c>
+      <c r="D232">
+        <f>VLOOKUP(A232,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A233" t="s">
+        <v>231</v>
+      </c>
+      <c r="B233">
+        <v>2</v>
+      </c>
+      <c r="D233">
+        <f>VLOOKUP(A233,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A234" t="s">
+        <v>226</v>
+      </c>
+      <c r="B234">
+        <v>2</v>
+      </c>
+      <c r="D234">
+        <f>VLOOKUP(A234,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A235" t="s">
+        <v>231</v>
+      </c>
+      <c r="B235">
+        <v>2</v>
+      </c>
+      <c r="D235">
+        <f>VLOOKUP(A235,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A236" t="s">
+        <v>226</v>
+      </c>
+      <c r="B236">
+        <v>2</v>
+      </c>
+      <c r="D236">
+        <f>VLOOKUP(A236,Sheet1!$A$2:$F$90,4,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated frequency to hex
</commit_message>
<xml_diff>
--- a/AVR 음악 주파수.xlsx
+++ b/AVR 음악 주파수.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WinAVR-RTOS\avr_rtos_orgel_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85847B11-2289-4454-AC1B-B3319D87360B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90E0637-1534-4ECC-8BA9-AB5C6F1CB0D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14976" activeTab="4" xr2:uid="{2A465206-010F-4655-81D6-FB1FD6055048}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14976" activeTab="6" xr2:uid="{2A465206-010F-4655-81D6-FB1FD6055048}"/>
   </bookViews>
   <sheets>
     <sheet name="코드표" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="238">
   <si>
     <t>B8</t>
   </si>
@@ -911,6 +911,14 @@
   </si>
   <si>
     <t>note_size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"0x" &amp; REPT("0", 2 - (LEN(DEC2HEX(K13)))) &amp; DEC2HEX(K13)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1661,8 +1669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446A7234-ADB2-406E-8008-66DD6109EBEE}">
   <dimension ref="A1:N109"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2355,9 +2363,8 @@
         <f t="shared" si="6"/>
         <v>255</v>
       </c>
-      <c r="L13" s="17" t="str">
-        <f t="shared" si="7"/>
-        <v>0xFF</v>
+      <c r="L13" s="17" t="s">
+        <v>236</v>
       </c>
       <c r="M13" s="12">
         <f t="shared" si="8"/>
@@ -11928,7 +11935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8B1577-E6D3-4CED-ABFA-BC6DADF1001D}">
   <dimension ref="A1:D236"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -14789,9 +14796,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213F771B-F8B9-4CDD-8BB3-B1EE240BB95C}">
   <dimension ref="A1:O90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" outlineLevelCol="1" x14ac:dyDescent="0.4"/>
@@ -14839,14 +14846,14 @@
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="K2">
-        <v>0</v>
+      <c r="K2" t="s">
+        <v>237</v>
       </c>
       <c r="L2" t="s">
         <v>186</v>
       </c>
-      <c r="N2">
-        <v>0</v>
+      <c r="N2" t="s">
+        <v>237</v>
       </c>
       <c r="O2" t="s">
         <v>186</v>
@@ -14865,14 +14872,16 @@
       <c r="F3">
         <v>243</v>
       </c>
-      <c r="K3">
-        <v>113</v>
+      <c r="K3" t="str">
+        <f>"0x" &amp; REPT("0", 2 - (LEN(DEC2HEX(E3)))) &amp; DEC2HEX(E3)</f>
+        <v>0x71</v>
       </c>
       <c r="L3" t="s">
         <v>186</v>
       </c>
-      <c r="N3">
-        <v>243</v>
+      <c r="N3" t="str">
+        <f>"0x" &amp; REPT("0", 2 - (LEN(DEC2HEX(F3)))) &amp; DEC2HEX(F3)</f>
+        <v>0xF3</v>
       </c>
       <c r="O3" t="s">
         <v>186</v>
@@ -14891,14 +14900,16 @@
       <c r="F4">
         <v>236</v>
       </c>
-      <c r="K4">
-        <v>121</v>
+      <c r="K4" t="str">
+        <f t="shared" ref="K4:K67" si="0">"0x" &amp; REPT("0", 2 - (LEN(DEC2HEX(E4)))) &amp; DEC2HEX(E4)</f>
+        <v>0x79</v>
       </c>
       <c r="L4" t="s">
         <v>186</v>
       </c>
-      <c r="N4">
-        <v>236</v>
+      <c r="N4" t="str">
+        <f t="shared" ref="N4:N67" si="1">"0x" &amp; REPT("0", 2 - (LEN(DEC2HEX(F4)))) &amp; DEC2HEX(F4)</f>
+        <v>0xEC</v>
       </c>
       <c r="O4" t="s">
         <v>186</v>
@@ -14917,14 +14928,16 @@
       <c r="F5">
         <v>115</v>
       </c>
-      <c r="K5">
-        <v>129</v>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>0x81</v>
       </c>
       <c r="L5" t="s">
         <v>186</v>
       </c>
-      <c r="N5">
-        <v>115</v>
+      <c r="N5" t="str">
+        <f t="shared" si="1"/>
+        <v>0x73</v>
       </c>
       <c r="O5" t="s">
         <v>186</v>
@@ -14943,14 +14956,16 @@
       <c r="F6">
         <v>141</v>
       </c>
-      <c r="K6">
-        <v>136</v>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>0x88</v>
       </c>
       <c r="L6" t="s">
         <v>186</v>
       </c>
-      <c r="N6">
-        <v>141</v>
+      <c r="N6" t="str">
+        <f t="shared" si="1"/>
+        <v>0x8D</v>
       </c>
       <c r="O6" t="s">
         <v>186</v>
@@ -14969,14 +14984,16 @@
       <c r="F7">
         <v>65</v>
       </c>
-      <c r="K7">
-        <v>143</v>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>0x8F</v>
       </c>
       <c r="L7" t="s">
         <v>186</v>
       </c>
-      <c r="N7">
-        <v>65</v>
+      <c r="N7" t="str">
+        <f t="shared" si="1"/>
+        <v>0x41</v>
       </c>
       <c r="O7" t="s">
         <v>186</v>
@@ -14995,14 +15012,16 @@
       <c r="F8">
         <v>149</v>
       </c>
-      <c r="K8">
-        <v>149</v>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>0x95</v>
       </c>
       <c r="L8" t="s">
         <v>186</v>
       </c>
-      <c r="N8">
-        <v>149</v>
+      <c r="N8" t="str">
+        <f t="shared" si="1"/>
+        <v>0x95</v>
       </c>
       <c r="O8" t="s">
         <v>186</v>
@@ -15021,14 +15040,16 @@
       <c r="F9">
         <v>142</v>
       </c>
-      <c r="K9">
-        <v>155</v>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>0x9B</v>
       </c>
       <c r="L9" t="s">
         <v>186</v>
       </c>
-      <c r="N9">
-        <v>142</v>
+      <c r="N9" t="str">
+        <f t="shared" si="1"/>
+        <v>0x8E</v>
       </c>
       <c r="O9" t="s">
         <v>186</v>
@@ -15047,14 +15068,16 @@
       <c r="F10">
         <v>49</v>
       </c>
-      <c r="K10">
-        <v>161</v>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>0xA1</v>
       </c>
       <c r="L10" t="s">
         <v>186</v>
       </c>
-      <c r="N10">
-        <v>49</v>
+      <c r="N10" t="str">
+        <f t="shared" si="1"/>
+        <v>0x31</v>
       </c>
       <c r="O10" t="s">
         <v>186</v>
@@ -15073,14 +15096,16 @@
       <c r="F11">
         <v>131</v>
       </c>
-      <c r="K11">
-        <v>166</v>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>0xA6</v>
       </c>
       <c r="L11" t="s">
         <v>186</v>
       </c>
-      <c r="N11">
-        <v>131</v>
+      <c r="N11" t="str">
+        <f t="shared" si="1"/>
+        <v>0x83</v>
       </c>
       <c r="O11" t="s">
         <v>186</v>
@@ -15099,14 +15124,16 @@
       <c r="F12">
         <v>137</v>
       </c>
-      <c r="K12">
-        <v>171</v>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>0xAB</v>
       </c>
       <c r="L12" t="s">
         <v>186</v>
       </c>
-      <c r="N12">
-        <v>137</v>
+      <c r="N12" t="str">
+        <f t="shared" si="1"/>
+        <v>0x89</v>
       </c>
       <c r="O12" t="s">
         <v>186</v>
@@ -15125,14 +15152,16 @@
       <c r="F13">
         <v>71</v>
       </c>
-      <c r="K13">
-        <v>176</v>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>0xB0</v>
       </c>
       <c r="L13" t="s">
         <v>186</v>
       </c>
-      <c r="N13">
-        <v>71</v>
+      <c r="N13" t="str">
+        <f t="shared" si="1"/>
+        <v>0x47</v>
       </c>
       <c r="O13" t="s">
         <v>186</v>
@@ -15151,14 +15180,16 @@
       <c r="F14">
         <v>192</v>
       </c>
-      <c r="K14">
-        <v>180</v>
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>0xB4</v>
       </c>
       <c r="L14" t="s">
         <v>186</v>
       </c>
-      <c r="N14">
-        <v>192</v>
+      <c r="N14" t="str">
+        <f t="shared" si="1"/>
+        <v>0xC0</v>
       </c>
       <c r="O14" t="s">
         <v>186</v>
@@ -15177,14 +15208,16 @@
       <c r="F15">
         <v>249</v>
       </c>
-      <c r="K15">
-        <v>184</v>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>0xB8</v>
       </c>
       <c r="L15" t="s">
         <v>186</v>
       </c>
-      <c r="N15">
-        <v>249</v>
+      <c r="N15" t="str">
+        <f t="shared" si="1"/>
+        <v>0xF9</v>
       </c>
       <c r="O15" t="s">
         <v>186</v>
@@ -15203,14 +15236,16 @@
       <c r="F16">
         <v>246</v>
       </c>
-      <c r="K16">
-        <v>188</v>
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>0xBC</v>
       </c>
       <c r="L16" t="s">
         <v>186</v>
       </c>
-      <c r="N16">
-        <v>246</v>
+      <c r="N16" t="str">
+        <f t="shared" si="1"/>
+        <v>0xF6</v>
       </c>
       <c r="O16" t="s">
         <v>186</v>
@@ -15229,14 +15264,16 @@
       <c r="F17">
         <v>185</v>
       </c>
-      <c r="K17">
-        <v>192</v>
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>0xC0</v>
       </c>
       <c r="L17" t="s">
         <v>186</v>
       </c>
-      <c r="N17">
-        <v>185</v>
+      <c r="N17" t="str">
+        <f t="shared" si="1"/>
+        <v>0xB9</v>
       </c>
       <c r="O17" t="s">
         <v>186</v>
@@ -15255,14 +15292,16 @@
       <c r="F18">
         <v>70</v>
       </c>
-      <c r="K18">
-        <v>196</v>
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>0xC4</v>
       </c>
       <c r="L18" t="s">
         <v>186</v>
       </c>
-      <c r="N18">
-        <v>70</v>
+      <c r="N18" t="str">
+        <f t="shared" si="1"/>
+        <v>0x46</v>
       </c>
       <c r="O18" t="s">
         <v>186</v>
@@ -15281,14 +15320,16 @@
       <c r="F19">
         <v>160</v>
       </c>
-      <c r="K19">
-        <v>199</v>
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v>0xC7</v>
       </c>
       <c r="L19" t="s">
         <v>186</v>
       </c>
-      <c r="N19">
-        <v>160</v>
+      <c r="N19" t="str">
+        <f t="shared" si="1"/>
+        <v>0xA0</v>
       </c>
       <c r="O19" t="s">
         <v>186</v>
@@ -15307,14 +15348,16 @@
       <c r="F20">
         <v>202</v>
       </c>
-      <c r="K20">
-        <v>202</v>
+      <c r="K20" t="str">
+        <f t="shared" si="0"/>
+        <v>0xCA</v>
       </c>
       <c r="L20" t="s">
         <v>186</v>
       </c>
-      <c r="N20">
-        <v>202</v>
+      <c r="N20" t="str">
+        <f t="shared" si="1"/>
+        <v>0xCA</v>
       </c>
       <c r="O20" t="s">
         <v>186</v>
@@ -15333,14 +15376,16 @@
       <c r="F21">
         <v>199</v>
       </c>
-      <c r="K21">
-        <v>205</v>
+      <c r="K21" t="str">
+        <f t="shared" si="0"/>
+        <v>0xCD</v>
       </c>
       <c r="L21" t="s">
         <v>186</v>
       </c>
-      <c r="N21">
-        <v>199</v>
+      <c r="N21" t="str">
+        <f t="shared" si="1"/>
+        <v>0xC7</v>
       </c>
       <c r="O21" t="s">
         <v>186</v>
@@ -15359,14 +15404,16 @@
       <c r="F22">
         <v>152</v>
       </c>
-      <c r="K22">
-        <v>208</v>
+      <c r="K22" t="str">
+        <f t="shared" si="0"/>
+        <v>0xD0</v>
       </c>
       <c r="L22" t="s">
         <v>186</v>
       </c>
-      <c r="N22">
-        <v>152</v>
+      <c r="N22" t="str">
+        <f t="shared" si="1"/>
+        <v>0x98</v>
       </c>
       <c r="O22" t="s">
         <v>186</v>
@@ -15385,14 +15432,16 @@
       <c r="F23">
         <v>65</v>
       </c>
-      <c r="K23">
-        <v>211</v>
+      <c r="K23" t="str">
+        <f t="shared" si="0"/>
+        <v>0xD3</v>
       </c>
       <c r="L23" t="s">
         <v>186</v>
       </c>
-      <c r="N23">
-        <v>65</v>
+      <c r="N23" t="str">
+        <f t="shared" si="1"/>
+        <v>0x41</v>
       </c>
       <c r="O23" t="s">
         <v>186</v>
@@ -15411,14 +15460,16 @@
       <c r="F24">
         <v>196</v>
       </c>
-      <c r="K24">
-        <v>213</v>
+      <c r="K24" t="str">
+        <f t="shared" si="0"/>
+        <v>0xD5</v>
       </c>
       <c r="L24" t="s">
         <v>186</v>
       </c>
-      <c r="N24">
-        <v>196</v>
+      <c r="N24" t="str">
+        <f t="shared" si="1"/>
+        <v>0xC4</v>
       </c>
       <c r="O24" t="s">
         <v>186</v>
@@ -15437,14 +15488,16 @@
       <c r="F25">
         <v>35</v>
       </c>
-      <c r="K25">
-        <v>216</v>
+      <c r="K25" t="str">
+        <f t="shared" si="0"/>
+        <v>0xD8</v>
       </c>
       <c r="L25" t="s">
         <v>186</v>
       </c>
-      <c r="N25">
-        <v>35</v>
+      <c r="N25" t="str">
+        <f t="shared" si="1"/>
+        <v>0x23</v>
       </c>
       <c r="O25" t="s">
         <v>186</v>
@@ -15463,14 +15516,16 @@
       <c r="F26">
         <v>96</v>
       </c>
-      <c r="K26">
-        <v>218</v>
+      <c r="K26" t="str">
+        <f t="shared" si="0"/>
+        <v>0xDA</v>
       </c>
       <c r="L26" t="s">
         <v>186</v>
       </c>
-      <c r="N26">
-        <v>96</v>
+      <c r="N26" t="str">
+        <f t="shared" si="1"/>
+        <v>0x60</v>
       </c>
       <c r="O26" t="s">
         <v>186</v>
@@ -15489,14 +15544,16 @@
       <c r="F27">
         <v>124</v>
       </c>
-      <c r="K27">
-        <v>220</v>
+      <c r="K27" t="str">
+        <f t="shared" si="0"/>
+        <v>0xDC</v>
       </c>
       <c r="L27" t="s">
         <v>186</v>
       </c>
-      <c r="N27">
-        <v>124</v>
+      <c r="N27" t="str">
+        <f t="shared" si="1"/>
+        <v>0x7C</v>
       </c>
       <c r="O27" t="s">
         <v>186</v>
@@ -15515,14 +15572,16 @@
       <c r="F28">
         <v>122</v>
       </c>
-      <c r="K28">
-        <v>222</v>
+      <c r="K28" t="str">
+        <f t="shared" si="0"/>
+        <v>0xDE</v>
       </c>
       <c r="L28" t="s">
         <v>186</v>
       </c>
-      <c r="N28">
-        <v>122</v>
+      <c r="N28" t="str">
+        <f t="shared" si="1"/>
+        <v>0x7A</v>
       </c>
       <c r="O28" t="s">
         <v>186</v>
@@ -15541,14 +15600,16 @@
       <c r="F29">
         <v>92</v>
       </c>
-      <c r="K29">
-        <v>224</v>
+      <c r="K29" t="str">
+        <f t="shared" si="0"/>
+        <v>0xE0</v>
       </c>
       <c r="L29" t="s">
         <v>186</v>
       </c>
-      <c r="N29">
-        <v>92</v>
+      <c r="N29" t="str">
+        <f t="shared" si="1"/>
+        <v>0x5C</v>
       </c>
       <c r="O29" t="s">
         <v>186</v>
@@ -15567,14 +15628,16 @@
       <c r="F30">
         <v>34</v>
       </c>
-      <c r="K30">
-        <v>226</v>
+      <c r="K30" t="str">
+        <f t="shared" si="0"/>
+        <v>0xE2</v>
       </c>
       <c r="L30" t="s">
         <v>186</v>
       </c>
-      <c r="N30">
-        <v>34</v>
+      <c r="N30" t="str">
+        <f t="shared" si="1"/>
+        <v>0x22</v>
       </c>
       <c r="O30" t="s">
         <v>186</v>
@@ -15593,14 +15656,16 @@
       <c r="F31">
         <v>208</v>
       </c>
-      <c r="K31">
-        <v>227</v>
+      <c r="K31" t="str">
+        <f t="shared" si="0"/>
+        <v>0xE3</v>
       </c>
       <c r="L31" t="s">
         <v>186</v>
       </c>
-      <c r="N31">
-        <v>208</v>
+      <c r="N31" t="str">
+        <f t="shared" si="1"/>
+        <v>0xD0</v>
       </c>
       <c r="O31" t="s">
         <v>186</v>
@@ -15619,14 +15684,16 @@
       <c r="F32">
         <v>101</v>
       </c>
-      <c r="K32">
-        <v>229</v>
+      <c r="K32" t="str">
+        <f t="shared" si="0"/>
+        <v>0xE5</v>
       </c>
       <c r="L32" t="s">
         <v>186</v>
       </c>
-      <c r="N32">
-        <v>101</v>
+      <c r="N32" t="str">
+        <f t="shared" si="1"/>
+        <v>0x65</v>
       </c>
       <c r="O32" t="s">
         <v>186</v>
@@ -15645,14 +15712,16 @@
       <c r="F33">
         <v>227</v>
       </c>
-      <c r="K33">
-        <v>230</v>
+      <c r="K33" t="str">
+        <f t="shared" si="0"/>
+        <v>0xE6</v>
       </c>
       <c r="L33" t="s">
         <v>186</v>
       </c>
-      <c r="N33">
-        <v>227</v>
+      <c r="N33" t="str">
+        <f t="shared" si="1"/>
+        <v>0xE3</v>
       </c>
       <c r="O33" t="s">
         <v>186</v>
@@ -15671,14 +15740,16 @@
       <c r="F34">
         <v>76</v>
       </c>
-      <c r="K34">
-        <v>232</v>
+      <c r="K34" t="str">
+        <f t="shared" si="0"/>
+        <v>0xE8</v>
       </c>
       <c r="L34" t="s">
         <v>186</v>
       </c>
-      <c r="N34">
-        <v>76</v>
+      <c r="N34" t="str">
+        <f t="shared" si="1"/>
+        <v>0x4C</v>
       </c>
       <c r="O34" t="s">
         <v>186</v>
@@ -15697,14 +15768,16 @@
       <c r="F35">
         <v>160</v>
       </c>
-      <c r="K35">
-        <v>233</v>
+      <c r="K35" t="str">
+        <f t="shared" si="0"/>
+        <v>0xE9</v>
       </c>
       <c r="L35" t="s">
         <v>186</v>
       </c>
-      <c r="N35">
-        <v>160</v>
+      <c r="N35" t="str">
+        <f t="shared" si="1"/>
+        <v>0xA0</v>
       </c>
       <c r="O35" t="s">
         <v>186</v>
@@ -15723,14 +15796,16 @@
       <c r="F36">
         <v>226</v>
       </c>
-      <c r="K36">
-        <v>234</v>
+      <c r="K36" t="str">
+        <f t="shared" si="0"/>
+        <v>0xEA</v>
       </c>
       <c r="L36" t="s">
         <v>186</v>
       </c>
-      <c r="N36">
-        <v>226</v>
+      <c r="N36" t="str">
+        <f t="shared" si="1"/>
+        <v>0xE2</v>
       </c>
       <c r="O36" t="s">
         <v>186</v>
@@ -15749,14 +15824,16 @@
       <c r="F37">
         <v>17</v>
       </c>
-      <c r="K37">
-        <v>236</v>
+      <c r="K37" t="str">
+        <f t="shared" si="0"/>
+        <v>0xEC</v>
       </c>
       <c r="L37" t="s">
         <v>186</v>
       </c>
-      <c r="N37">
-        <v>17</v>
+      <c r="N37" t="str">
+        <f t="shared" si="1"/>
+        <v>0x11</v>
       </c>
       <c r="O37" t="s">
         <v>186</v>
@@ -15775,14 +15852,16 @@
       <c r="F38">
         <v>47</v>
       </c>
-      <c r="K38">
-        <v>237</v>
+      <c r="K38" t="str">
+        <f t="shared" si="0"/>
+        <v>0xED</v>
       </c>
       <c r="L38" t="s">
         <v>186</v>
       </c>
-      <c r="N38">
-        <v>47</v>
+      <c r="N38" t="str">
+        <f t="shared" si="1"/>
+        <v>0x2F</v>
       </c>
       <c r="O38" t="s">
         <v>186</v>
@@ -15801,14 +15880,16 @@
       <c r="F39">
         <v>62</v>
       </c>
-      <c r="K39">
-        <v>238</v>
+      <c r="K39" t="str">
+        <f t="shared" si="0"/>
+        <v>0xEE</v>
       </c>
       <c r="L39" t="s">
         <v>186</v>
       </c>
-      <c r="N39">
-        <v>62</v>
+      <c r="N39" t="str">
+        <f t="shared" si="1"/>
+        <v>0x3E</v>
       </c>
       <c r="O39" t="s">
         <v>186</v>
@@ -15827,14 +15908,16 @@
       <c r="F40">
         <v>61</v>
       </c>
-      <c r="K40">
-        <v>239</v>
+      <c r="K40" t="str">
+        <f t="shared" si="0"/>
+        <v>0xEF</v>
       </c>
       <c r="L40" t="s">
         <v>186</v>
       </c>
-      <c r="N40">
-        <v>61</v>
+      <c r="N40" t="str">
+        <f t="shared" si="1"/>
+        <v>0x3D</v>
       </c>
       <c r="O40" t="s">
         <v>186</v>
@@ -15853,14 +15936,16 @@
       <c r="F41">
         <v>45</v>
       </c>
-      <c r="K41">
-        <v>240</v>
+      <c r="K41" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF0</v>
       </c>
       <c r="L41" t="s">
         <v>186</v>
       </c>
-      <c r="N41">
-        <v>45</v>
+      <c r="N41" t="str">
+        <f t="shared" si="1"/>
+        <v>0x2D</v>
       </c>
       <c r="O41" t="s">
         <v>186</v>
@@ -15879,14 +15964,16 @@
       <c r="F42">
         <v>17</v>
       </c>
-      <c r="K42">
-        <v>241</v>
+      <c r="K42" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF1</v>
       </c>
       <c r="L42" t="s">
         <v>186</v>
       </c>
-      <c r="N42">
-        <v>17</v>
+      <c r="N42" t="str">
+        <f t="shared" si="1"/>
+        <v>0x11</v>
       </c>
       <c r="O42" t="s">
         <v>186</v>
@@ -15905,14 +15992,16 @@
       <c r="F43">
         <v>231</v>
       </c>
-      <c r="K43">
-        <v>241</v>
+      <c r="K43" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF1</v>
       </c>
       <c r="L43" t="s">
         <v>186</v>
       </c>
-      <c r="N43">
-        <v>231</v>
+      <c r="N43" t="str">
+        <f t="shared" si="1"/>
+        <v>0xE7</v>
       </c>
       <c r="O43" t="s">
         <v>186</v>
@@ -15931,14 +16020,16 @@
       <c r="F44">
         <v>178</v>
       </c>
-      <c r="K44">
-        <v>242</v>
+      <c r="K44" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF2</v>
       </c>
       <c r="L44" t="s">
         <v>186</v>
       </c>
-      <c r="N44">
-        <v>178</v>
+      <c r="N44" t="str">
+        <f t="shared" si="1"/>
+        <v>0xB2</v>
       </c>
       <c r="O44" t="s">
         <v>186</v>
@@ -15957,14 +16048,16 @@
       <c r="F45">
         <v>113</v>
       </c>
-      <c r="K45">
-        <v>243</v>
+      <c r="K45" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF3</v>
       </c>
       <c r="L45" t="s">
         <v>186</v>
       </c>
-      <c r="N45">
-        <v>113</v>
+      <c r="N45" t="str">
+        <f t="shared" si="1"/>
+        <v>0x71</v>
       </c>
       <c r="O45" t="s">
         <v>186</v>
@@ -15983,14 +16076,16 @@
       <c r="F46">
         <v>37</v>
       </c>
-      <c r="K46">
-        <v>244</v>
+      <c r="K46" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF4</v>
       </c>
       <c r="L46" t="s">
         <v>186</v>
       </c>
-      <c r="N46">
-        <v>37</v>
+      <c r="N46" t="str">
+        <f t="shared" si="1"/>
+        <v>0x25</v>
       </c>
       <c r="O46" t="s">
         <v>186</v>
@@ -16009,14 +16104,16 @@
       <c r="F47">
         <v>208</v>
       </c>
-      <c r="K47">
-        <v>244</v>
+      <c r="K47" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF4</v>
       </c>
       <c r="L47" t="s">
         <v>186</v>
       </c>
-      <c r="N47">
-        <v>208</v>
+      <c r="N47" t="str">
+        <f t="shared" si="1"/>
+        <v>0xD0</v>
       </c>
       <c r="O47" t="s">
         <v>186</v>
@@ -16035,14 +16132,16 @@
       <c r="F48">
         <v>112</v>
       </c>
-      <c r="K48">
-        <v>245</v>
+      <c r="K48" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF5</v>
       </c>
       <c r="L48" t="s">
         <v>186</v>
       </c>
-      <c r="N48">
-        <v>112</v>
+      <c r="N48" t="str">
+        <f t="shared" si="1"/>
+        <v>0x70</v>
       </c>
       <c r="O48" t="s">
         <v>186</v>
@@ -16061,14 +16160,16 @@
       <c r="F49">
         <v>8</v>
       </c>
-      <c r="K49">
-        <v>246</v>
+      <c r="K49" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF6</v>
       </c>
       <c r="L49" t="s">
         <v>186</v>
       </c>
-      <c r="N49">
-        <v>8</v>
+      <c r="N49" t="str">
+        <f t="shared" si="1"/>
+        <v>0x08</v>
       </c>
       <c r="O49" t="s">
         <v>186</v>
@@ -16087,14 +16188,16 @@
       <c r="F50">
         <v>151</v>
       </c>
-      <c r="K50">
-        <v>246</v>
+      <c r="K50" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF6</v>
       </c>
       <c r="L50" t="s">
         <v>186</v>
       </c>
-      <c r="N50">
-        <v>151</v>
+      <c r="N50" t="str">
+        <f t="shared" si="1"/>
+        <v>0x97</v>
       </c>
       <c r="O50" t="s">
         <v>186</v>
@@ -16113,14 +16216,16 @@
       <c r="F51">
         <v>30</v>
       </c>
-      <c r="K51">
-        <v>247</v>
+      <c r="K51" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF7</v>
       </c>
       <c r="L51" t="s">
         <v>186</v>
       </c>
-      <c r="N51">
-        <v>30</v>
+      <c r="N51" t="str">
+        <f t="shared" si="1"/>
+        <v>0x1E</v>
       </c>
       <c r="O51" t="s">
         <v>186</v>
@@ -16139,14 +16244,16 @@
       <c r="F52">
         <v>158</v>
       </c>
-      <c r="K52">
-        <v>247</v>
+      <c r="K52" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF7</v>
       </c>
       <c r="L52" t="s">
         <v>186</v>
       </c>
-      <c r="N52">
-        <v>158</v>
+      <c r="N52" t="str">
+        <f t="shared" si="1"/>
+        <v>0x9E</v>
       </c>
       <c r="O52" t="s">
         <v>186</v>
@@ -16165,14 +16272,16 @@
       <c r="F53">
         <v>22</v>
       </c>
-      <c r="K53">
-        <v>248</v>
+      <c r="K53" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF8</v>
       </c>
       <c r="L53" t="s">
         <v>186</v>
       </c>
-      <c r="N53">
-        <v>22</v>
+      <c r="N53" t="str">
+        <f t="shared" si="1"/>
+        <v>0x16</v>
       </c>
       <c r="O53" t="s">
         <v>186</v>
@@ -16191,14 +16300,16 @@
       <c r="F54">
         <v>136</v>
       </c>
-      <c r="K54">
-        <v>248</v>
+      <c r="K54" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF8</v>
       </c>
       <c r="L54" t="s">
         <v>186</v>
       </c>
-      <c r="N54">
-        <v>136</v>
+      <c r="N54" t="str">
+        <f t="shared" si="1"/>
+        <v>0x88</v>
       </c>
       <c r="O54" t="s">
         <v>186</v>
@@ -16217,14 +16328,16 @@
       <c r="F55">
         <v>243</v>
       </c>
-      <c r="K55">
-        <v>248</v>
+      <c r="K55" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF8</v>
       </c>
       <c r="L55" t="s">
         <v>186</v>
       </c>
-      <c r="N55">
-        <v>243</v>
+      <c r="N55" t="str">
+        <f t="shared" si="1"/>
+        <v>0xF3</v>
       </c>
       <c r="O55" t="s">
         <v>186</v>
@@ -16243,14 +16356,16 @@
       <c r="F56">
         <v>88</v>
       </c>
-      <c r="K56">
-        <v>249</v>
+      <c r="K56" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF9</v>
       </c>
       <c r="L56" t="s">
         <v>186</v>
       </c>
-      <c r="N56">
-        <v>88</v>
+      <c r="N56" t="str">
+        <f t="shared" si="1"/>
+        <v>0x58</v>
       </c>
       <c r="O56" t="s">
         <v>186</v>
@@ -16269,14 +16384,16 @@
       <c r="F57">
         <v>184</v>
       </c>
-      <c r="K57">
-        <v>249</v>
+      <c r="K57" t="str">
+        <f t="shared" si="0"/>
+        <v>0xF9</v>
       </c>
       <c r="L57" t="s">
         <v>186</v>
       </c>
-      <c r="N57">
-        <v>184</v>
+      <c r="N57" t="str">
+        <f t="shared" si="1"/>
+        <v>0xB8</v>
       </c>
       <c r="O57" t="s">
         <v>186</v>
@@ -16295,14 +16412,16 @@
       <c r="F58">
         <v>18</v>
       </c>
-      <c r="K58">
-        <v>250</v>
+      <c r="K58" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFA</v>
       </c>
       <c r="L58" t="s">
         <v>186</v>
       </c>
-      <c r="N58">
-        <v>18</v>
+      <c r="N58" t="str">
+        <f t="shared" si="1"/>
+        <v>0x12</v>
       </c>
       <c r="O58" t="s">
         <v>186</v>
@@ -16321,14 +16440,16 @@
       <c r="F59">
         <v>103</v>
       </c>
-      <c r="K59">
-        <v>250</v>
+      <c r="K59" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFA</v>
       </c>
       <c r="L59" t="s">
         <v>186</v>
       </c>
-      <c r="N59">
-        <v>103</v>
+      <c r="N59" t="str">
+        <f t="shared" si="1"/>
+        <v>0x67</v>
       </c>
       <c r="O59" t="s">
         <v>186</v>
@@ -16347,14 +16468,16 @@
       <c r="F60">
         <v>184</v>
       </c>
-      <c r="K60">
-        <v>250</v>
+      <c r="K60" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFA</v>
       </c>
       <c r="L60" t="s">
         <v>186</v>
       </c>
-      <c r="N60">
-        <v>184</v>
+      <c r="N60" t="str">
+        <f t="shared" si="1"/>
+        <v>0xB8</v>
       </c>
       <c r="O60" t="s">
         <v>186</v>
@@ -16373,14 +16496,16 @@
       <c r="F61">
         <v>3</v>
       </c>
-      <c r="K61">
-        <v>251</v>
+      <c r="K61" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFB</v>
       </c>
       <c r="L61" t="s">
         <v>186</v>
       </c>
-      <c r="N61">
-        <v>3</v>
+      <c r="N61" t="str">
+        <f t="shared" si="1"/>
+        <v>0x03</v>
       </c>
       <c r="O61" t="s">
         <v>186</v>
@@ -16399,14 +16524,16 @@
       <c r="F62">
         <v>75</v>
       </c>
-      <c r="K62">
-        <v>251</v>
+      <c r="K62" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFB</v>
       </c>
       <c r="L62" t="s">
         <v>186</v>
       </c>
-      <c r="N62">
-        <v>75</v>
+      <c r="N62" t="str">
+        <f t="shared" si="1"/>
+        <v>0x4B</v>
       </c>
       <c r="O62" t="s">
         <v>186</v>
@@ -16425,14 +16552,16 @@
       <c r="F63">
         <v>143</v>
       </c>
-      <c r="K63">
-        <v>251</v>
+      <c r="K63" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFB</v>
       </c>
       <c r="L63" t="s">
         <v>186</v>
       </c>
-      <c r="N63">
-        <v>143</v>
+      <c r="N63" t="str">
+        <f t="shared" si="1"/>
+        <v>0x8F</v>
       </c>
       <c r="O63" t="s">
         <v>186</v>
@@ -16451,14 +16580,16 @@
       <c r="F64">
         <v>206</v>
       </c>
-      <c r="K64">
-        <v>251</v>
+      <c r="K64" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFB</v>
       </c>
       <c r="L64" t="s">
         <v>186</v>
       </c>
-      <c r="N64">
-        <v>206</v>
+      <c r="N64" t="str">
+        <f t="shared" si="1"/>
+        <v>0xCE</v>
       </c>
       <c r="O64" t="s">
         <v>186</v>
@@ -16483,14 +16614,16 @@
       <c r="F65">
         <v>11</v>
       </c>
-      <c r="K65">
-        <v>252</v>
+      <c r="K65" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFC</v>
       </c>
       <c r="L65" t="s">
         <v>186</v>
       </c>
-      <c r="N65">
-        <v>11</v>
+      <c r="N65" t="str">
+        <f t="shared" si="1"/>
+        <v>0x0B</v>
       </c>
       <c r="O65" t="s">
         <v>186</v>
@@ -16515,14 +16648,16 @@
       <c r="F66">
         <v>67</v>
       </c>
-      <c r="K66">
-        <v>252</v>
+      <c r="K66" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFC</v>
       </c>
       <c r="L66" t="s">
         <v>186</v>
       </c>
-      <c r="N66">
-        <v>67</v>
+      <c r="N66" t="str">
+        <f t="shared" si="1"/>
+        <v>0x43</v>
       </c>
       <c r="O66" t="s">
         <v>186</v>
@@ -16547,14 +16682,16 @@
       <c r="F67">
         <v>121</v>
       </c>
-      <c r="K67">
-        <v>252</v>
+      <c r="K67" t="str">
+        <f t="shared" si="0"/>
+        <v>0xFC</v>
       </c>
       <c r="L67" t="s">
         <v>186</v>
       </c>
-      <c r="N67">
-        <v>121</v>
+      <c r="N67" t="str">
+        <f t="shared" si="1"/>
+        <v>0x79</v>
       </c>
       <c r="O67" t="s">
         <v>186</v>
@@ -16579,14 +16716,16 @@
       <c r="F68">
         <v>172</v>
       </c>
-      <c r="K68">
-        <v>252</v>
+      <c r="K68" t="str">
+        <f t="shared" ref="K68:K90" si="2">"0x" &amp; REPT("0", 2 - (LEN(DEC2HEX(E68)))) &amp; DEC2HEX(E68)</f>
+        <v>0xFC</v>
       </c>
       <c r="L68" t="s">
         <v>186</v>
       </c>
-      <c r="N68">
-        <v>172</v>
+      <c r="N68" t="str">
+        <f t="shared" ref="N68:N89" si="3">"0x" &amp; REPT("0", 2 - (LEN(DEC2HEX(F68)))) &amp; DEC2HEX(F68)</f>
+        <v>0xAC</v>
       </c>
       <c r="O68" t="s">
         <v>186</v>
@@ -16611,14 +16750,16 @@
       <c r="F69">
         <v>219</v>
       </c>
-      <c r="K69">
-        <v>252</v>
+      <c r="K69" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFC</v>
       </c>
       <c r="L69" t="s">
         <v>186</v>
       </c>
-      <c r="N69">
-        <v>219</v>
+      <c r="N69" t="str">
+        <f t="shared" si="3"/>
+        <v>0xDB</v>
       </c>
       <c r="O69" t="s">
         <v>186</v>
@@ -16643,14 +16784,16 @@
       <c r="F70">
         <v>9</v>
       </c>
-      <c r="K70">
-        <v>253</v>
+      <c r="K70" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFD</v>
       </c>
       <c r="L70" t="s">
         <v>186</v>
       </c>
-      <c r="N70">
-        <v>9</v>
+      <c r="N70" t="str">
+        <f t="shared" si="3"/>
+        <v>0x09</v>
       </c>
       <c r="O70" t="s">
         <v>186</v>
@@ -16675,14 +16818,16 @@
       <c r="F71">
         <v>51</v>
       </c>
-      <c r="K71">
-        <v>253</v>
+      <c r="K71" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFD</v>
       </c>
       <c r="L71" t="s">
         <v>186</v>
       </c>
-      <c r="N71">
-        <v>51</v>
+      <c r="N71" t="str">
+        <f t="shared" si="3"/>
+        <v>0x33</v>
       </c>
       <c r="O71" t="s">
         <v>186</v>
@@ -16707,14 +16852,16 @@
       <c r="F72">
         <v>91</v>
       </c>
-      <c r="K72">
-        <v>253</v>
+      <c r="K72" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFD</v>
       </c>
       <c r="L72" t="s">
         <v>186</v>
       </c>
-      <c r="N72">
-        <v>91</v>
+      <c r="N72" t="str">
+        <f t="shared" si="3"/>
+        <v>0x5B</v>
       </c>
       <c r="O72" t="s">
         <v>186</v>
@@ -16739,14 +16886,16 @@
       <c r="F73">
         <v>129</v>
       </c>
-      <c r="K73">
-        <v>253</v>
+      <c r="K73" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFD</v>
       </c>
       <c r="L73" t="s">
         <v>186</v>
       </c>
-      <c r="N73">
-        <v>129</v>
+      <c r="N73" t="str">
+        <f t="shared" si="3"/>
+        <v>0x81</v>
       </c>
       <c r="O73" t="s">
         <v>186</v>
@@ -16771,14 +16920,16 @@
       <c r="F74">
         <v>165</v>
       </c>
-      <c r="K74">
-        <v>253</v>
+      <c r="K74" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFD</v>
       </c>
       <c r="L74" t="s">
         <v>186</v>
       </c>
-      <c r="N74">
-        <v>165</v>
+      <c r="N74" t="str">
+        <f t="shared" si="3"/>
+        <v>0xA5</v>
       </c>
       <c r="O74" t="s">
         <v>186</v>
@@ -16803,14 +16954,16 @@
       <c r="F75">
         <v>199</v>
       </c>
-      <c r="K75">
-        <v>253</v>
+      <c r="K75" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFD</v>
       </c>
       <c r="L75" t="s">
         <v>186</v>
       </c>
-      <c r="N75">
-        <v>199</v>
+      <c r="N75" t="str">
+        <f t="shared" si="3"/>
+        <v>0xC7</v>
       </c>
       <c r="O75" t="s">
         <v>186</v>
@@ -16835,14 +16988,16 @@
       <c r="F76">
         <v>231</v>
       </c>
-      <c r="K76">
-        <v>253</v>
+      <c r="K76" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFD</v>
       </c>
       <c r="L76" t="s">
         <v>186</v>
       </c>
-      <c r="N76">
-        <v>231</v>
+      <c r="N76" t="str">
+        <f t="shared" si="3"/>
+        <v>0xE7</v>
       </c>
       <c r="O76" t="s">
         <v>186</v>
@@ -16867,14 +17022,16 @@
       <c r="F77">
         <v>5</v>
       </c>
-      <c r="K77">
-        <v>254</v>
+      <c r="K77" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFE</v>
       </c>
       <c r="L77" t="s">
         <v>186</v>
       </c>
-      <c r="N77">
-        <v>5</v>
+      <c r="N77" t="str">
+        <f t="shared" si="3"/>
+        <v>0x05</v>
       </c>
       <c r="O77" t="s">
         <v>186</v>
@@ -16899,14 +17056,16 @@
       <c r="F78">
         <v>33</v>
       </c>
-      <c r="K78">
-        <v>254</v>
+      <c r="K78" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFE</v>
       </c>
       <c r="L78" t="s">
         <v>186</v>
       </c>
-      <c r="N78">
-        <v>33</v>
+      <c r="N78" t="str">
+        <f t="shared" si="3"/>
+        <v>0x21</v>
       </c>
       <c r="O78" t="s">
         <v>186</v>
@@ -16931,14 +17090,16 @@
       <c r="F79">
         <v>60</v>
       </c>
-      <c r="K79">
-        <v>254</v>
+      <c r="K79" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFE</v>
       </c>
       <c r="L79" t="s">
         <v>186</v>
       </c>
-      <c r="N79">
-        <v>60</v>
+      <c r="N79" t="str">
+        <f t="shared" si="3"/>
+        <v>0x3C</v>
       </c>
       <c r="O79" t="s">
         <v>186</v>
@@ -16963,14 +17124,16 @@
       <c r="F80">
         <v>85</v>
       </c>
-      <c r="K80">
-        <v>254</v>
+      <c r="K80" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFE</v>
       </c>
       <c r="L80" t="s">
         <v>186</v>
       </c>
-      <c r="N80">
-        <v>85</v>
+      <c r="N80" t="str">
+        <f t="shared" si="3"/>
+        <v>0x55</v>
       </c>
       <c r="O80" t="s">
         <v>186</v>
@@ -16995,14 +17158,16 @@
       <c r="F81">
         <v>109</v>
       </c>
-      <c r="K81">
-        <v>254</v>
+      <c r="K81" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFE</v>
       </c>
       <c r="L81" t="s">
         <v>186</v>
       </c>
-      <c r="N81">
-        <v>109</v>
+      <c r="N81" t="str">
+        <f t="shared" si="3"/>
+        <v>0x6D</v>
       </c>
       <c r="O81" t="s">
         <v>186</v>
@@ -17027,14 +17192,16 @@
       <c r="F82">
         <v>132</v>
       </c>
-      <c r="K82">
-        <v>254</v>
+      <c r="K82" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFE</v>
       </c>
       <c r="L82" t="s">
         <v>186</v>
       </c>
-      <c r="N82">
-        <v>132</v>
+      <c r="N82" t="str">
+        <f t="shared" si="3"/>
+        <v>0x84</v>
       </c>
       <c r="O82" t="s">
         <v>186</v>
@@ -17059,14 +17226,16 @@
       <c r="F83">
         <v>153</v>
       </c>
-      <c r="K83">
-        <v>254</v>
+      <c r="K83" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFE</v>
       </c>
       <c r="L83" t="s">
         <v>186</v>
       </c>
-      <c r="N83">
-        <v>153</v>
+      <c r="N83" t="str">
+        <f t="shared" si="3"/>
+        <v>0x99</v>
       </c>
       <c r="O83" t="s">
         <v>186</v>
@@ -17091,14 +17260,16 @@
       <c r="F84">
         <v>173</v>
       </c>
-      <c r="K84">
-        <v>254</v>
+      <c r="K84" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFE</v>
       </c>
       <c r="L84" t="s">
         <v>186</v>
       </c>
-      <c r="N84">
-        <v>173</v>
+      <c r="N84" t="str">
+        <f t="shared" si="3"/>
+        <v>0xAD</v>
       </c>
       <c r="O84" t="s">
         <v>186</v>
@@ -17123,14 +17294,16 @@
       <c r="F85">
         <v>192</v>
       </c>
-      <c r="K85">
-        <v>254</v>
+      <c r="K85" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFE</v>
       </c>
       <c r="L85" t="s">
         <v>186</v>
       </c>
-      <c r="N85">
-        <v>192</v>
+      <c r="N85" t="str">
+        <f t="shared" si="3"/>
+        <v>0xC0</v>
       </c>
       <c r="O85" t="s">
         <v>186</v>
@@ -17155,14 +17328,16 @@
       <c r="F86">
         <v>210</v>
       </c>
-      <c r="K86">
-        <v>254</v>
+      <c r="K86" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFE</v>
       </c>
       <c r="L86" t="s">
         <v>186</v>
       </c>
-      <c r="N86">
-        <v>210</v>
+      <c r="N86" t="str">
+        <f t="shared" si="3"/>
+        <v>0xD2</v>
       </c>
       <c r="O86" t="s">
         <v>186</v>
@@ -17187,14 +17362,16 @@
       <c r="F87">
         <v>227</v>
       </c>
-      <c r="K87">
-        <v>254</v>
+      <c r="K87" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFE</v>
       </c>
       <c r="L87" t="s">
         <v>186</v>
       </c>
-      <c r="N87">
-        <v>227</v>
+      <c r="N87" t="str">
+        <f t="shared" si="3"/>
+        <v>0xE3</v>
       </c>
       <c r="O87" t="s">
         <v>186</v>
@@ -17219,14 +17396,16 @@
       <c r="F88">
         <v>243</v>
       </c>
-      <c r="K88">
-        <v>254</v>
+      <c r="K88" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFE</v>
       </c>
       <c r="L88" t="s">
         <v>186</v>
       </c>
-      <c r="N88">
-        <v>243</v>
+      <c r="N88" t="str">
+        <f t="shared" si="3"/>
+        <v>0xF3</v>
       </c>
       <c r="O88" t="s">
         <v>186</v>
@@ -17251,14 +17430,16 @@
       <c r="F89">
         <v>2</v>
       </c>
-      <c r="K89">
-        <v>255</v>
+      <c r="K89" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFF</v>
       </c>
       <c r="L89" t="s">
         <v>186</v>
       </c>
-      <c r="N89">
-        <v>2</v>
+      <c r="N89" t="str">
+        <f t="shared" si="3"/>
+        <v>0x02</v>
       </c>
       <c r="O89" t="s">
         <v>186</v>
@@ -17283,14 +17464,16 @@
       <c r="F90">
         <v>16</v>
       </c>
-      <c r="K90">
-        <v>255</v>
+      <c r="K90" t="str">
+        <f t="shared" si="2"/>
+        <v>0xFF</v>
       </c>
       <c r="L90" t="s">
         <v>186</v>
       </c>
-      <c r="N90">
-        <v>16</v>
+      <c r="N90" t="str">
+        <f>"0x" &amp; REPT("0", 2 - (LEN(DEC2HEX(F90)))) &amp; DEC2HEX(F90)</f>
+        <v>0x10</v>
       </c>
       <c r="O90" t="s">
         <v>186</v>
@@ -17300,5 +17483,6 @@
   <autoFilter ref="A1:F1" xr:uid="{6A5B7B47-DD28-4E07-BCAB-138231999424}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated some things and added new task
</commit_message>
<xml_diff>
--- a/AVR 음악 주파수.xlsx
+++ b/AVR 음악 주파수.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WinAVR-RTOS\avr_rtos_orgel_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2385252B-2D12-4CF8-8B58-31B22EC5D8A2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86138393-37EA-49BA-9BE6-6FD2B887FEF2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14976" activeTab="2" xr2:uid="{2A465206-010F-4655-81D6-FB1FD6055048}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14976" activeTab="1" xr2:uid="{2A465206-010F-4655-81D6-FB1FD6055048}"/>
   </bookViews>
   <sheets>
     <sheet name="코드표" sheetId="1" r:id="rId1"/>
@@ -7157,7 +7157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{792AC214-B357-4346-80DB-EF2DB51532C2}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -8418,8 +8418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF3DE661-5C59-4E79-89C9-E5FEDDE2D563}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="I1:J54"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -9994,6 +9994,10 @@
       <c r="B55">
         <f>SUM(B1:B54)</f>
         <v>144</v>
+      </c>
+      <c r="C55">
+        <f>SUM(C1:C54)</f>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -10005,10 +10009,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37FA565B-722B-41B4-AC68-8ECC1B03CA2F}">
-  <dimension ref="A1:F154"/>
+  <dimension ref="A1:F155"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B155" sqref="B155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -12467,6 +12471,12 @@
       <c r="F154">
         <f t="shared" si="2"/>
         <v>52</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B155">
+        <f>SUM(B2:B154)</f>
+        <v>770</v>
       </c>
     </row>
   </sheetData>
@@ -12478,10 +12488,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8B1577-E6D3-4CED-ABFA-BC6DADF1001D}">
-  <dimension ref="A1:D236"/>
+  <dimension ref="A1:D237"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="B237" sqref="B237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -15315,6 +15325,12 @@
       <c r="D236">
         <f>VLOOKUP(A236,Sheet1!$A$2:$F$90,4,FALSE)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B237">
+        <f>SUM(B2:B236)</f>
+        <v>750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>